<commit_message>
[Update] Skill csv & xlsx
</commit_message>
<xml_diff>
--- a/Documents/Files/Skill.xlsx
+++ b/Documents/Files/Skill.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sparta_Coding_Club\TeamProject\TextRPG_TeamProject2nd\TextRPG_TeamProject2nd\Documents\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2FEC01-494A-4E20-B668-30340B77290E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250E9572-DF8B-4205-9055-5443F20BA3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -367,11 +367,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>자신의 주위를 어둠으로 둘러, 체력을 대량으로 회복한다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>온 몸을 비틀며 몸의 형상을 정돈한다. 체력을 매우 크게 회복한다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>자신의 주위를 어둠으로 둘러 체력을 대량으로 회복한다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -724,7 +724,7 @@
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1179,7 +1179,7 @@
         <v>38</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="4">
         <v>100</v>
@@ -1219,7 +1219,7 @@
         <v>34</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24" s="4">
         <v>70</v>

</xml_diff>